<commit_message>
enabled passing ids of nodes instead of json, restructured the project
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFD0DAF-9269-445F-8ED1-3D92FA2E1D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53177977-10DF-41D7-840C-E77DC2A19DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -346,9 +346,6 @@
     <t>["X","y"]</t>
   </si>
   <si>
-    <t>evluator</t>
-  </si>
-  <si>
     <t>metric</t>
   </si>
   <si>
@@ -1006,6 +1003,9 @@
   </si>
   <si>
     <t>[{"name":"shape","type":"list","default":[1,1]}]</t>
+  </si>
+  <si>
+    <t>evaluator</t>
   </si>
 </sst>
 </file>
@@ -1422,8 +1422,8 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1443,16 +1443,16 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1467,10 +1467,10 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>83</v>
@@ -1478,16 +1478,16 @@
     </row>
     <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
@@ -1508,21 +1508,21 @@
         <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>23</v>
@@ -1543,21 +1543,21 @@
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
@@ -1578,21 +1578,21 @@
         <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
@@ -1613,21 +1613,21 @@
         <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -1648,21 +1648,21 @@
         <v>5</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>19</v>
@@ -1683,21 +1683,21 @@
         <v>5</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
@@ -1718,21 +1718,21 @@
         <v>5</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
@@ -1753,24 +1753,24 @@
         <v>5</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
@@ -1788,21 +1788,21 @@
         <v>5</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>11</v>
@@ -1823,21 +1823,21 @@
         <v>5</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>12</v>
@@ -1858,21 +1858,21 @@
         <v>5</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>13</v>
@@ -1893,24 +1893,24 @@
         <v>5</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1928,21 +1928,21 @@
         <v>5</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>14</v>
@@ -1963,21 +1963,21 @@
         <v>5</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>15</v>
@@ -1998,21 +1998,21 @@
         <v>5</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>16</v>
@@ -2024,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>4</v>
@@ -2033,21 +2033,21 @@
         <v>5</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>91</v>
@@ -2059,7 +2059,7 @@
         <v>7</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>4</v>
@@ -2068,21 +2068,21 @@
         <v>5</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>92</v>
@@ -2094,7 +2094,7 @@
         <v>8</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>4</v>
@@ -2103,21 +2103,21 @@
         <v>5</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>90</v>
@@ -2138,21 +2138,21 @@
         <v>5</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>89</v>
@@ -2173,21 +2173,21 @@
         <v>5</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>84</v>
@@ -2208,21 +2208,21 @@
         <v>5</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>85</v>
@@ -2243,21 +2243,21 @@
         <v>5</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>86</v>
@@ -2278,21 +2278,21 @@
         <v>5</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>87</v>
@@ -2313,24 +2313,24 @@
         <v>5</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>29</v>
@@ -2348,21 +2348,21 @@
         <v>5</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>88</v>
@@ -2383,21 +2383,21 @@
         <v>5</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>30</v>
@@ -2418,21 +2418,21 @@
         <v>5</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>31</v>
@@ -2453,21 +2453,21 @@
         <v>5</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>32</v>
@@ -2488,21 +2488,21 @@
         <v>5</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>33</v>
@@ -2523,21 +2523,21 @@
         <v>5</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>34</v>
@@ -2558,21 +2558,21 @@
         <v>5</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>39</v>
@@ -2593,21 +2593,21 @@
         <v>75</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>40</v>
@@ -2628,21 +2628,21 @@
         <v>75</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C35" s="1">
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>41</v>
@@ -2663,21 +2663,21 @@
         <v>75</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>42</v>
@@ -2698,21 +2698,21 @@
         <v>75</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C37" s="1">
         <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>43</v>
@@ -2733,21 +2733,21 @@
         <v>75</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>49</v>
@@ -2768,21 +2768,21 @@
         <v>75</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>50</v>
@@ -2803,21 +2803,21 @@
         <v>75</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C40" s="1">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>51</v>
@@ -2838,21 +2838,21 @@
         <v>75</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C41" s="1">
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>52</v>
@@ -2873,21 +2873,21 @@
         <v>75</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C42" s="1">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>56</v>
@@ -2908,21 +2908,21 @@
         <v>75</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>57</v>
@@ -2943,21 +2943,21 @@
         <v>75</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C44" s="1">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>54</v>
@@ -2978,21 +2978,21 @@
         <v>75</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C45" s="1">
         <v>4</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>61</v>
@@ -3001,33 +3001,33 @@
         <v>62</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>79</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C46" s="1">
         <v>4</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>63</v>
@@ -3042,27 +3042,27 @@
         <v>4</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" s="1">
         <v>4</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>65</v>
@@ -3071,7 +3071,7 @@
         <v>62</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>4</v>
@@ -3083,27 +3083,27 @@
         <v>78</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C48" s="1">
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>66</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>67</v>
@@ -3118,27 +3118,27 @@
         <v>70</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C49" s="1">
         <v>4</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>68</v>
@@ -3150,30 +3150,30 @@
         <v>81</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C50" s="1">
         <v>6</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>72</v>
@@ -3188,30 +3188,30 @@
         <v>76</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>4</v>
@@ -3223,27 +3223,27 @@
         <v>100</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>93</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>94</v>
@@ -3258,27 +3258,27 @@
         <v>4</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>97</v>
@@ -3293,27 +3293,27 @@
         <v>95</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C54" s="1">
         <v>6</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>99</v>
@@ -3322,62 +3322,62 @@
         <v>4</v>
       </c>
       <c r="I54" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J54" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K54" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C55" s="1">
         <v>4</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E55" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="K55" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C56" s="1">
         <v>4</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>58</v>
@@ -3398,252 +3398,252 @@
         <v>74</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="C57" s="1">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J57" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="K57" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C58" s="1">
         <v>5</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C59" s="1">
         <v>5</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C60" s="1">
         <v>5</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C61" s="1">
+        <v>5</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C61" s="1">
-        <v>5</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="G61" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H61" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="H61" s="4" t="s">
+      <c r="I61" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="J61" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="K61" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C62" s="1">
         <v>5</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C63" s="1">
         <v>5</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="E63" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="F63" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="H63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added logs to chatbot
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DB6490-640A-4779-BE79-D8CFD3A07978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79252FA8-824F-4281-9C2E-B26D03632ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="315">
   <si>
     <t>node_name</t>
   </si>
@@ -1046,7 +1046,11 @@
   </si>
   <si>
     <t>[{"name":"optimizer","type":"str","default":"adam","choices":["adam","sgd","adamax","adamw","rmsprop"]}, {"name":"loss","type":"str","default":"categorical_crossentropy","choices":["categorical_crossentropy","mean_squared_error","binary_crossentropy","sparse_categorical_crossentropy"]},
-{"name":"metrics","type":"list","default":"accuracy","choices":["accuracy","mse","mae"]}]</t>
+{"name":"metrics","type":"list","default":["accuracy"],"choices":["accuracy","mse","mae"]}]</t>
+  </si>
+  <si>
+    <t>[{"name":"batch_size", "type":"int", "default":10},
+{"name":"epochs", "type":"int", "default":10}]</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1489,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H65" sqref="H65"/>
+      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3743,7 +3747,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>307</v>
       </c>
@@ -3766,7 +3770,7 @@
         <v>129</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>4</v>
+        <v>314</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>312</v>

</xml_diff>

<commit_message>
added uid column to node table
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A840FD-3F05-46AD-B650-B7F947C45F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F88EE8D-A96E-4138-9564-82078A51FBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="315">
   <si>
     <t>node_name</t>
   </si>
@@ -226,16 +226,10 @@
     <t>preprocessor_fitter</t>
   </si>
   <si>
-    <t>data_transformer</t>
-  </si>
-  <si>
     <t>transform</t>
   </si>
   <si>
     <t>fit_transform</t>
-  </si>
-  <si>
-    <t>fit_transformer</t>
   </si>
   <si>
     <t>["transformed_data"]</t>
@@ -1502,9 +1496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1524,19 +1518,19 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -1551,13 +1545,13 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1565,16 +1559,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>24</v>
@@ -1595,7 +1589,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1603,16 +1597,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
@@ -1633,7 +1627,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1641,16 +1635,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>22</v>
@@ -1671,7 +1665,7 @@
         <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1679,16 +1673,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
@@ -1709,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1717,16 +1711,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>20</v>
@@ -1738,7 +1732,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>4</v>
@@ -1747,7 +1741,7 @@
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1755,16 +1749,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>19</v>
@@ -1776,7 +1770,7 @@
         <v>8</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>4</v>
@@ -1785,7 +1779,7 @@
         <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -1793,16 +1787,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>18</v>
@@ -1823,7 +1817,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1831,16 +1825,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
@@ -1852,7 +1846,7 @@
         <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>4</v>
@@ -1861,7 +1855,7 @@
         <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1869,19 +1863,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>9</v>
@@ -1899,7 +1893,7 @@
         <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -1907,16 +1901,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>11</v>
@@ -1937,7 +1931,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1945,16 +1939,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>12</v>
@@ -1975,7 +1969,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1983,16 +1977,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>13</v>
@@ -2013,7 +2007,7 @@
         <v>5</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2021,19 +2015,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>9</v>
@@ -2051,7 +2045,7 @@
         <v>5</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2059,16 +2053,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>14</v>
@@ -2089,7 +2083,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2097,16 +2091,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
@@ -2127,7 +2121,7 @@
         <v>5</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2135,16 +2129,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>16</v>
@@ -2165,7 +2159,7 @@
         <v>5</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2173,19 +2167,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>27</v>
@@ -2194,7 +2188,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>4</v>
@@ -2203,7 +2197,7 @@
         <v>5</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2211,19 +2205,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>27</v>
@@ -2232,7 +2226,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>4</v>
@@ -2241,7 +2235,7 @@
         <v>5</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2249,19 +2243,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>27</v>
@@ -2270,7 +2264,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>4</v>
@@ -2279,7 +2273,7 @@
         <v>5</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -2287,19 +2281,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>27</v>
@@ -2308,7 +2302,7 @@
         <v>8</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>4</v>
@@ -2317,7 +2311,7 @@
         <v>5</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2325,19 +2319,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>27</v>
@@ -2355,7 +2349,7 @@
         <v>5</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2363,19 +2357,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>27</v>
@@ -2393,7 +2387,7 @@
         <v>5</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2401,19 +2395,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>27</v>
@@ -2431,7 +2425,7 @@
         <v>5</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -2439,19 +2433,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>27</v>
@@ -2469,7 +2463,7 @@
         <v>5</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2477,19 +2471,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>27</v>
@@ -2507,7 +2501,7 @@
         <v>5</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2515,19 +2509,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>27</v>
@@ -2545,7 +2539,7 @@
         <v>5</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2553,16 +2547,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>28</v>
@@ -2583,7 +2577,7 @@
         <v>5</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2591,16 +2585,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>29</v>
@@ -2621,7 +2615,7 @@
         <v>5</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2629,16 +2623,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>30</v>
@@ -2659,7 +2653,7 @@
         <v>5</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2667,16 +2661,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>31</v>
@@ -2697,7 +2691,7 @@
         <v>5</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2705,16 +2699,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D32" s="1">
         <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>32</v>
@@ -2735,7 +2729,7 @@
         <v>5</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2743,16 +2737,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D33" s="1">
         <v>3</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>37</v>
@@ -2770,10 +2764,10 @@
         <v>4</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2781,16 +2775,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D34" s="1">
         <v>3</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>38</v>
@@ -2808,10 +2802,10 @@
         <v>4</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2819,16 +2813,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D35" s="1">
         <v>3</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>39</v>
@@ -2846,10 +2840,10 @@
         <v>4</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2857,16 +2851,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D36" s="1">
         <v>3</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>40</v>
@@ -2884,10 +2878,10 @@
         <v>4</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2895,16 +2889,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D37" s="1">
         <v>3</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>41</v>
@@ -2916,16 +2910,16 @@
         <v>42</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2933,16 +2927,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>45</v>
@@ -2960,10 +2954,10 @@
         <v>4</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2971,16 +2965,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>46</v>
@@ -2998,10 +2992,10 @@
         <v>4</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -3009,16 +3003,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>47</v>
@@ -3036,10 +3030,10 @@
         <v>4</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3047,16 +3041,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D41" s="1">
         <v>3</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>48</v>
@@ -3074,10 +3068,10 @@
         <v>4</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3085,16 +3079,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D42" s="1">
         <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>52</v>
@@ -3112,10 +3106,10 @@
         <v>4</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3123,16 +3117,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D43" s="1">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>53</v>
@@ -3150,10 +3144,10 @@
         <v>4</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3161,16 +3155,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D44" s="1">
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>50</v>
@@ -3188,10 +3182,10 @@
         <v>4</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3199,16 +3193,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D45" s="1">
         <v>4</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>57</v>
@@ -3217,19 +3211,19 @@
         <v>58</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3237,16 +3231,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D46" s="1">
         <v>4</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>59</v>
@@ -3261,13 +3255,13 @@
         <v>4</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3275,16 +3269,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D47" s="1">
         <v>4</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>61</v>
@@ -3293,19 +3287,19 @@
         <v>58</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3313,37 +3307,37 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D48" s="1">
         <v>4</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="I48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3351,37 +3345,37 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D49" s="1">
         <v>4</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3389,25 +3383,25 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D50" s="1">
         <v>6</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>4</v>
@@ -3416,10 +3410,10 @@
         <v>56</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3427,37 +3421,37 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3465,37 +3459,37 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F52" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="K52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3503,37 +3497,37 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3541,37 +3535,37 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D54" s="1">
         <v>6</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K54" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3579,37 +3573,37 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D55" s="1">
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="J55" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I55" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="L55" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3617,25 +3611,25 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D56" s="1">
         <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>55</v>
@@ -3644,10 +3638,10 @@
         <v>56</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
@@ -3655,37 +3649,37 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D57" s="1">
+        <v>5</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="D57" s="1">
-        <v>5</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>257</v>
-      </c>
       <c r="G57" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="L57" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="L57" s="6" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
@@ -3693,37 +3687,37 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D58" s="1">
         <v>5</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G58" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="I58" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3731,37 +3725,37 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D59" s="1">
         <v>5</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G59" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="I59" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
@@ -3769,37 +3763,37 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D60" s="1">
         <v>5</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G60" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="I60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3807,37 +3801,37 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="D61" s="1">
         <v>5</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G61" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="I61" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K61" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="L61" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3845,37 +3839,37 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D62" s="1">
         <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G62" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="I62" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
@@ -3883,37 +3877,37 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D63" s="1">
         <v>5</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G63" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="K63" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -3921,37 +3915,37 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D64" s="1">
+        <v>5</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="G64" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D64" s="1">
-        <v>5</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F64" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="I64" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K64" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="L64" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3959,37 +3953,37 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="D65" s="7">
+        <v>5</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F65" s="9" t="s">
         <v>302</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="D65" s="7">
-        <v>5</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>304</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>58</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K65" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
train_test_split logic change it takes X, y and returns two sets each set is consisted of train and test data (they can be splitted using splitter node). ----- enhanced logic of repository layer ----- added unittests of model fitter, predictor, evaluator
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F88EE8D-A96E-4138-9564-82078A51FBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DC0D46-7C7D-4246-A95B-CFEABC33A374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="316">
   <si>
     <t>node_name</t>
   </si>
@@ -204,10 +204,6 @@
     <t>train_test_split</t>
   </si>
   <si>
-    <t xml:space="preserve">[{"name":"  "test_size","type":"float","default":0.3},    
-{"name":" random_state", "type":"float", "default":42}] </t>
-  </si>
-  <si>
     <t>["data"]</t>
   </si>
   <si>
@@ -242,9 +238,6 @@
   </si>
   <si>
     <t>data_loader</t>
-  </si>
-  <si>
-    <t>["train_data","test_data"]</t>
   </si>
   <si>
     <t>["preprocessor"]</t>
@@ -1052,6 +1045,16 @@
   </si>
   <si>
     <t>[{"name":"node_path", "type":"str", "default":""}]</t>
+  </si>
+  <si>
+    <t>["X", "y"]</t>
+  </si>
+  <si>
+    <t>["X_Split","y_Split"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"name": "test_size","type":"float","default":0.3},    
+{"name":" random_state", "type":"float", "default":42}] </t>
   </si>
 </sst>
 </file>
@@ -1496,9 +1499,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1518,19 +1521,19 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -1545,13 +1548,13 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1559,16 +1562,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>24</v>
@@ -1589,7 +1592,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1597,16 +1600,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
@@ -1627,7 +1630,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1635,16 +1638,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>22</v>
@@ -1665,7 +1668,7 @@
         <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1673,16 +1676,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
@@ -1703,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1711,16 +1714,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>20</v>
@@ -1732,7 +1735,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>4</v>
@@ -1741,7 +1744,7 @@
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1749,16 +1752,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>19</v>
@@ -1770,7 +1773,7 @@
         <v>8</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>4</v>
@@ -1779,7 +1782,7 @@
         <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -1787,16 +1790,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>18</v>
@@ -1817,7 +1820,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1825,16 +1828,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
@@ -1846,7 +1849,7 @@
         <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>4</v>
@@ -1855,7 +1858,7 @@
         <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1863,19 +1866,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>9</v>
@@ -1893,7 +1896,7 @@
         <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -1901,16 +1904,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>11</v>
@@ -1931,7 +1934,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1939,16 +1942,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>12</v>
@@ -1969,7 +1972,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1977,16 +1980,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>13</v>
@@ -2007,7 +2010,7 @@
         <v>5</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2015,19 +2018,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>9</v>
@@ -2045,7 +2048,7 @@
         <v>5</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2053,16 +2056,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>14</v>
@@ -2083,7 +2086,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2091,16 +2094,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
@@ -2121,7 +2124,7 @@
         <v>5</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2129,16 +2132,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>16</v>
@@ -2159,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2167,19 +2170,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>27</v>
@@ -2188,7 +2191,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>4</v>
@@ -2197,7 +2200,7 @@
         <v>5</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2205,19 +2208,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>27</v>
@@ -2226,7 +2229,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>4</v>
@@ -2235,7 +2238,7 @@
         <v>5</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2243,19 +2246,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>27</v>
@@ -2264,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>4</v>
@@ -2273,7 +2276,7 @@
         <v>5</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -2281,19 +2284,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>27</v>
@@ -2302,7 +2305,7 @@
         <v>8</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>4</v>
@@ -2311,7 +2314,7 @@
         <v>5</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2319,19 +2322,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>27</v>
@@ -2349,7 +2352,7 @@
         <v>5</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2357,19 +2360,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>27</v>
@@ -2387,7 +2390,7 @@
         <v>5</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2395,19 +2398,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>27</v>
@@ -2425,7 +2428,7 @@
         <v>5</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -2433,19 +2436,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>27</v>
@@ -2463,7 +2466,7 @@
         <v>5</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2471,19 +2474,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>27</v>
@@ -2501,7 +2504,7 @@
         <v>5</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2509,19 +2512,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>27</v>
@@ -2539,7 +2542,7 @@
         <v>5</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2547,16 +2550,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>28</v>
@@ -2577,7 +2580,7 @@
         <v>5</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2585,16 +2588,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>29</v>
@@ -2615,7 +2618,7 @@
         <v>5</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2623,16 +2626,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>30</v>
@@ -2653,7 +2656,7 @@
         <v>5</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2661,16 +2664,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>31</v>
@@ -2691,7 +2694,7 @@
         <v>5</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2699,16 +2702,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D32" s="1">
         <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>32</v>
@@ -2729,7 +2732,7 @@
         <v>5</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2737,16 +2740,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D33" s="1">
         <v>3</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>37</v>
@@ -2764,10 +2767,10 @@
         <v>4</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2775,16 +2778,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D34" s="1">
         <v>3</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>38</v>
@@ -2802,10 +2805,10 @@
         <v>4</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2813,16 +2816,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D35" s="1">
         <v>3</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>39</v>
@@ -2840,10 +2843,10 @@
         <v>4</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2851,16 +2854,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D36" s="1">
         <v>3</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>40</v>
@@ -2878,10 +2881,10 @@
         <v>4</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2889,16 +2892,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D37" s="1">
         <v>3</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>41</v>
@@ -2910,16 +2913,16 @@
         <v>42</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2927,16 +2930,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>45</v>
@@ -2954,10 +2957,10 @@
         <v>4</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2965,16 +2968,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>46</v>
@@ -2992,10 +2995,10 @@
         <v>4</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -3003,16 +3006,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>47</v>
@@ -3030,10 +3033,10 @@
         <v>4</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3041,16 +3044,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D41" s="1">
         <v>3</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>48</v>
@@ -3068,10 +3071,10 @@
         <v>4</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3079,16 +3082,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D42" s="1">
         <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>52</v>
@@ -3106,10 +3109,10 @@
         <v>4</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3117,16 +3120,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D43" s="1">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>53</v>
@@ -3144,10 +3147,10 @@
         <v>4</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3155,16 +3158,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D44" s="1">
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>50</v>
@@ -3182,10 +3185,10 @@
         <v>4</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3193,37 +3196,37 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D45" s="1">
         <v>4</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="H45" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3231,37 +3234,37 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D46" s="1">
         <v>4</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="I46" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3269,37 +3272,37 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D47" s="1">
         <v>4</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3307,37 +3310,37 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D48" s="1">
         <v>4</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3345,37 +3348,37 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D49" s="1">
         <v>4</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3383,37 +3386,37 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D50" s="1">
         <v>6</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F50" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="I50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3421,37 +3424,37 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3459,37 +3462,37 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F52" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="K52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3497,37 +3500,37 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3535,37 +3538,37 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D54" s="1">
         <v>6</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G54" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="K54" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3573,37 +3576,37 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D55" s="1">
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="J55" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I55" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="L55" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3611,37 +3614,37 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D56" s="1">
         <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G56" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="I56" s="4" t="s">
-        <v>55</v>
+        <v>315</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>56</v>
+        <v>313</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>68</v>
+        <v>314</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
@@ -3649,37 +3652,37 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D57" s="1">
+        <v>5</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D57" s="1">
-        <v>5</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>255</v>
-      </c>
       <c r="G57" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="L57" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="L57" s="6" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
@@ -3687,37 +3690,37 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D58" s="1">
         <v>5</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G58" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="I58" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -3725,37 +3728,37 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D59" s="1">
         <v>5</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G59" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="I59" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
@@ -3763,37 +3766,37 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D60" s="1">
         <v>5</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G60" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="I60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3801,37 +3804,37 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="D61" s="1">
         <v>5</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G61" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="I61" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K61" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="L61" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3839,37 +3842,37 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D62" s="1">
         <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G62" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="I62" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
@@ -3877,37 +3880,37 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D63" s="1">
         <v>5</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G63" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="K63" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -3915,37 +3918,37 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D64" s="1">
+        <v>5</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="G64" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D64" s="1">
-        <v>5</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F64" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="I64" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="K64" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="L64" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3953,37 +3956,37 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D65" s="7">
+        <v>5</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="F65" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="G65" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="K65" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="D65" s="7">
-        <v>5</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="F65" s="9" t="s">
+      <c r="L65" s="7" t="s">
         <v>302</v>
-      </c>
-      <c r="G65" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I65" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="J65" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="K65" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="L65" s="7" t="s">
-        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete unnecessary code lines
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DC0D46-7C7D-4246-A95B-CFEABC33A374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A61634-D42F-405D-A577-89966964E864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -1040,13 +1040,6 @@
     <t>uid</t>
   </si>
   <si>
-    <t>[{"name":"dataset_name","type":"str","default":"iris", "choices": ["iris","digits","diabetes","make_regression","make_classification"]},
-{"name":"dataset_path", "type":"str", "default":""}]</t>
-  </si>
-  <si>
-    <t>[{"name":"node_path", "type":"str", "default":""}]</t>
-  </si>
-  <si>
     <t>["X", "y"]</t>
   </si>
   <si>
@@ -1055,6 +1048,13 @@
   <si>
     <t xml:space="preserve">[{"name": "test_size","type":"float","default":0.3},    
 {"name":" random_state", "type":"float", "default":42}] </t>
+  </si>
+  <si>
+    <t>[{"name":"dataset_name","type":"str","default":"iris", "choices": ["iris","digits","diabetes","make_regression","make_classification"]},
+{"name":"dataset_path", "type":"path", "default":"", "extensions":["pkl", "csv", "xlsx"]}]</t>
+  </si>
+  <si>
+    <t>[{"name":"node_path", "type":"path", "default":"", "extensions":["pkl"]}]</t>
   </si>
 </sst>
 </file>
@@ -1500,8 +1500,8 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3445,7 +3445,7 @@
         <v>103</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>4</v>
@@ -3521,7 +3521,7 @@
         <v>89</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>4</v>
@@ -3635,13 +3635,13 @@
         <v>65</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
make the line curvey
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A61634-D42F-405D-A577-89966964E864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5B932D-8D4F-4735-8708-2BD6CF0E25CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -1046,15 +1046,15 @@
     <t>["X_Split","y_Split"]</t>
   </si>
   <si>
-    <t xml:space="preserve">[{"name": "test_size","type":"float","default":0.3},    
-{"name":" random_state", "type":"float", "default":42}] </t>
-  </si>
-  <si>
     <t>[{"name":"dataset_name","type":"str","default":"iris", "choices": ["iris","digits","diabetes","make_regression","make_classification"]},
 {"name":"dataset_path", "type":"path", "default":"", "extensions":["pkl", "csv", "xlsx"]}]</t>
   </si>
   <si>
     <t>[{"name":"node_path", "type":"path", "default":"", "extensions":["pkl"]}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"name": "test_size","type":"float","default":0.3},    
+{"name":" random_state", "type":"int", "default":42}] </t>
   </si>
 </sst>
 </file>
@@ -1500,8 +1500,8 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3445,7 +3445,7 @@
         <v>103</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>4</v>
@@ -3521,7 +3521,7 @@
         <v>89</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>4</v>
@@ -3635,7 +3635,7 @@
         <v>65</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>311</v>

</xml_diff>

<commit_message>
updated serializers, views fixed bugs related to node saver, node loader
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A61634-D42F-405D-A577-89966964E864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379D6371-BC30-48D1-A5BA-0D4E21C24CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="318">
   <si>
     <t>node_name</t>
   </si>
@@ -966,10 +966,6 @@
   </si>
   <si>
     <t>[{"name":"metric", "type":"str","default":"accuracy", "choices":["f1","r2","recall","mse","accuracy","mae","precision","log_loss","rmse"]}]</t>
-  </si>
-  <si>
-    <t>[{"name":"units","type":"int","default":1},
-{"name":"activation","type":"str","default":"relu",  "choices":["relu", "linear", "sigmoid", "leaky_relu", "tanh"]}]</t>
   </si>
   <si>
     <t>Network Compiler</t>
@@ -1046,15 +1042,25 @@
     <t>["X_Split","y_Split"]</t>
   </si>
   <si>
-    <t xml:space="preserve">[{"name": "test_size","type":"float","default":0.3},    
-{"name":" random_state", "type":"float", "default":42}] </t>
-  </si>
-  <si>
     <t>[{"name":"dataset_name","type":"str","default":"iris", "choices": ["iris","digits","diabetes","make_regression","make_classification"]},
 {"name":"dataset_path", "type":"path", "default":"", "extensions":["pkl", "csv", "xlsx"]}]</t>
   </si>
   <si>
     <t>[{"name":"node_path", "type":"path", "default":"", "extensions":["pkl"]}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"name": "test_size","type":"float","default":0.3},    
+{"name":" random_state", "type":"int", "default":42}] </t>
+  </si>
+  <si>
+    <t>[{"name":"units","type":"int","default":1},
+{"name":"activation","type":"str","default":"relu",  "choices":["relu", "linear", "sigmoid", "leaky_relu", "tanh", "softmax"]}]</t>
+  </si>
+  <si>
+    <t>[{"name":"node_path", "type":"path", "default": ""}]</t>
+  </si>
+  <si>
+    <t>[""]</t>
   </si>
 </sst>
 </file>
@@ -1499,9 +1505,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1521,7 +1527,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>126</v>
@@ -2913,7 +2919,7 @@
         <v>42</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>4</v>
@@ -3445,7 +3451,7 @@
         <v>103</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>4</v>
@@ -3483,13 +3489,13 @@
         <v>86</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>4</v>
+        <v>316</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>87</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>4</v>
+        <v>317</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>116</v>
@@ -3521,7 +3527,7 @@
         <v>89</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>4</v>
@@ -3635,13 +3641,13 @@
         <v>65</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="J56" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="K56" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>120</v>
@@ -3673,7 +3679,7 @@
         <v>262</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>4</v>
@@ -3711,7 +3717,7 @@
         <v>262</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>268</v>
@@ -3749,7 +3755,7 @@
         <v>262</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>268</v>
@@ -3825,7 +3831,7 @@
         <v>262</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>268</v>
@@ -3918,10 +3924,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="D64" s="1">
         <v>5</v>
@@ -3930,25 +3936,25 @@
         <v>255</v>
       </c>
       <c r="F64" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="I64" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>267</v>
       </c>
       <c r="K64" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="L64" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -3956,10 +3962,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>299</v>
       </c>
       <c r="D65" s="7">
         <v>5</v>
@@ -3968,7 +3974,7 @@
         <v>255</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>57</v>
@@ -3977,16 +3983,16 @@
         <v>124</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K65" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="L65" s="7" t="s">
         <v>301</v>
-      </c>
-      <c r="L65" s="7" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated schema node_saver, loader
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379D6371-BC30-48D1-A5BA-0D4E21C24CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78628FE-43AB-4086-8320-E467D50BEEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -1046,9 +1046,6 @@
 {"name":"dataset_path", "type":"path", "default":"", "extensions":["pkl", "csv", "xlsx"]}]</t>
   </si>
   <si>
-    <t>[{"name":"node_path", "type":"path", "default":"", "extensions":["pkl"]}]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[{"name": "test_size","type":"float","default":0.3},    
 {"name":" random_state", "type":"int", "default":42}] </t>
   </si>
@@ -1057,10 +1054,13 @@
 {"name":"activation","type":"str","default":"relu",  "choices":["relu", "linear", "sigmoid", "leaky_relu", "tanh", "softmax"]}]</t>
   </si>
   <si>
-    <t>[{"name":"node_path", "type":"path", "default": ""}]</t>
-  </si>
-  <si>
     <t>[""]</t>
+  </si>
+  <si>
+    <t>[{"name":"node_path", "type":"path_folder", "default": ""}]</t>
+  </si>
+  <si>
+    <t>[{"name":"node_path", "type":"path_file", "default":"", "extensions":["pkl"]}]</t>
   </si>
 </sst>
 </file>
@@ -1505,9 +1505,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3495,7 +3495,7 @@
         <v>87</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>116</v>
@@ -3527,7 +3527,7 @@
         <v>89</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>4</v>
@@ -3641,7 +3641,7 @@
         <v>65</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>310</v>
@@ -3831,7 +3831,7 @@
         <v>262</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>268</v>

</xml_diff>

<commit_message>
- AI assistant can detect whether the user want to chat or execute an aino pipeline - fixed node connection bug - added locations for each created node to help chatbot.
</commit_message>
<xml_diff>
--- a/project/core/schema.xlsx
+++ b/project/core/schema.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4258,6 +4258,114 @@
         </is>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>a new one</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>a new one</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>6</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Custom</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>a_new_one</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>custom</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>template</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>['node']</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>template/</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>a brand new node</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>a brand new node description</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>6</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Custom</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>a_brand_new_node</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>custom</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>template</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>[{'penalty': 'l2'}, {'C': 1.0}]</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>['node']</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>template/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>